<commit_message>
Anexo las funciones de regresion lineal por partes
</commit_message>
<xml_diff>
--- a/Dataset/DatosSiembraPromedios.xlsx
+++ b/Dataset/DatosSiembraPromedios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\LabModeMat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\maizmodelo\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A05A6D3F-D445-4F2A-9AE9-4F3551A0E274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35335A80-914C-4AA8-BE1F-9E62F02F9628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5205737B-CB3A-45F4-B54E-3D176AF54BDB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{5205737B-CB3A-45F4-B54E-3D176AF54BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">	PRECIP</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>DIAS</t>
+  </si>
+  <si>
+    <t>HI</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,8 +114,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -135,11 +144,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,12 +176,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DF6202-73D5-4282-97C2-BEA4A57586A0}">
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +522,7 @@
     <col min="6" max="6" width="13.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -499,8 +541,11 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" cm="1">
         <f t="array" ref="A2:A216">_xlfn.SEQUENCE(COUNT(B:B))</f>
         <v>1</v>
@@ -520,8 +565,11 @@
       <c r="F2" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -540,8 +588,11 @@
       <c r="F3" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -560,8 +611,11 @@
       <c r="F4" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -580,8 +634,11 @@
       <c r="F5" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -600,8 +657,11 @@
       <c r="F6" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -620,8 +680,11 @@
       <c r="F7" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -640,8 +703,11 @@
       <c r="F8" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -660,8 +726,11 @@
       <c r="F9" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -680,8 +749,11 @@
       <c r="F10" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -700,8 +772,11 @@
       <c r="F11" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -720,8 +795,11 @@
       <c r="F12" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="8">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -740,8 +818,11 @@
       <c r="F13" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -760,8 +841,11 @@
       <c r="F14" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -780,8 +864,11 @@
       <c r="F15" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -800,8 +887,11 @@
       <c r="F16" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="6">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -820,8 +910,11 @@
       <c r="F17" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="6">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -840,8 +933,11 @@
       <c r="F18" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="6">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -860,8 +956,11 @@
       <c r="F19" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -880,8 +979,11 @@
       <c r="F20" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="6">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -900,8 +1002,11 @@
       <c r="F21" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -920,8 +1025,11 @@
       <c r="F22" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="6">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -940,8 +1048,11 @@
       <c r="F23" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="6">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -960,8 +1071,11 @@
       <c r="F24" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="6">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -980,8 +1094,11 @@
       <c r="F25" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1000,8 +1117,11 @@
       <c r="F26" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="6">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1020,8 +1140,11 @@
       <c r="F27" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="6">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1040,8 +1163,11 @@
       <c r="F28" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="6">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1060,8 +1186,11 @@
       <c r="F29" s="3">
         <v>12.833333333333334</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="6">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1080,8 +1209,11 @@
       <c r="F30" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="6">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1100,8 +1232,11 @@
       <c r="F31" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="6">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1120,8 +1255,11 @@
       <c r="F32" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1140,8 +1278,11 @@
       <c r="F33" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="6">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1160,8 +1301,11 @@
       <c r="F34" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="6">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1180,8 +1324,11 @@
       <c r="F35" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="6">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1200,8 +1347,11 @@
       <c r="F36" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="6">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1220,8 +1370,11 @@
       <c r="F37" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="6">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1240,8 +1393,11 @@
       <c r="F38" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="6">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1260,8 +1416,11 @@
       <c r="F39" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="6">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1280,8 +1439,11 @@
       <c r="F40" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="6">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1300,8 +1462,11 @@
       <c r="F41" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="6">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1320,8 +1485,11 @@
       <c r="F42" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="6">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1340,8 +1508,11 @@
       <c r="F43" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="6">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1360,8 +1531,11 @@
       <c r="F44" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="6">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1380,8 +1554,11 @@
       <c r="F45" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1400,8 +1577,11 @@
       <c r="F46" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="6">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1420,8 +1600,11 @@
       <c r="F47" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="6">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1440,8 +1623,11 @@
       <c r="F48" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="6">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1460,8 +1646,11 @@
       <c r="F49" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="6">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1480,8 +1669,11 @@
       <c r="F50" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="6">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1500,8 +1692,11 @@
       <c r="F51" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="6">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1520,8 +1715,11 @@
       <c r="F52" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="6">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1540,8 +1738,11 @@
       <c r="F53" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="6">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1560,8 +1761,11 @@
       <c r="F54" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1580,8 +1784,11 @@
       <c r="F55" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="7">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1600,8 +1807,11 @@
       <c r="F56" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" s="7">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1620,8 +1830,11 @@
       <c r="F57" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="7">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1640,8 +1853,11 @@
       <c r="F58" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1660,8 +1876,11 @@
       <c r="F59" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1680,8 +1899,11 @@
       <c r="F60" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1700,8 +1922,11 @@
       <c r="F61" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>38.799999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1720,8 +1945,11 @@
       <c r="F62" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>39.700000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1740,8 +1968,11 @@
       <c r="F63" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1760,8 +1991,11 @@
       <c r="F64" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1780,8 +2014,11 @@
       <c r="F65" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1800,8 +2037,11 @@
       <c r="F66" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1820,8 +2060,11 @@
       <c r="F67" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1840,8 +2083,11 @@
       <c r="F68" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1860,8 +2106,11 @@
       <c r="F69" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69">
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1880,8 +2129,11 @@
       <c r="F70" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70">
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1900,8 +2152,11 @@
       <c r="F71" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1920,8 +2175,11 @@
       <c r="F72" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1940,8 +2198,11 @@
       <c r="F73" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1960,8 +2221,11 @@
       <c r="F74" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1980,8 +2244,11 @@
       <c r="F75" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2000,8 +2267,11 @@
       <c r="F76" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2020,8 +2290,11 @@
       <c r="F77" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2040,8 +2313,11 @@
       <c r="F78" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2060,8 +2336,11 @@
       <c r="F79" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2080,8 +2359,11 @@
       <c r="F80" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2100,8 +2382,11 @@
       <c r="F81" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2120,8 +2405,11 @@
       <c r="F82" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2140,8 +2428,11 @@
       <c r="F83" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2160,8 +2451,11 @@
       <c r="F84" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2180,8 +2474,11 @@
       <c r="F85" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2200,8 +2497,11 @@
       <c r="F86" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2220,8 +2520,11 @@
       <c r="F87" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2240,8 +2543,11 @@
       <c r="F88" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2260,8 +2566,11 @@
       <c r="F89" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2280,8 +2589,11 @@
       <c r="F90" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2300,8 +2612,11 @@
       <c r="F91" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2320,8 +2635,11 @@
       <c r="F92" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2340,8 +2658,11 @@
       <c r="F93" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2360,8 +2681,11 @@
       <c r="F94" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2380,8 +2704,11 @@
       <c r="F95" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2400,8 +2727,11 @@
       <c r="F96" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2420,8 +2750,11 @@
       <c r="F97" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2440,8 +2773,11 @@
       <c r="F98" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2460,8 +2796,11 @@
       <c r="F99" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2480,8 +2819,11 @@
       <c r="F100" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2500,8 +2842,11 @@
       <c r="F101" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2520,8 +2865,11 @@
       <c r="F102" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2540,8 +2888,11 @@
       <c r="F103" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G103">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2560,8 +2911,11 @@
       <c r="F104" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G104">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2580,8 +2934,11 @@
       <c r="F105" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G105">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2600,8 +2957,11 @@
       <c r="F106" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G106">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2620,8 +2980,11 @@
       <c r="F107" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G107">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2640,8 +3003,11 @@
       <c r="F108" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G108">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2660,8 +3026,11 @@
       <c r="F109" s="3">
         <v>12.333333333333334</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G109">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2680,8 +3049,11 @@
       <c r="F110" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2700,8 +3072,11 @@
       <c r="F111" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G111">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2720,8 +3095,11 @@
       <c r="F112" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G112">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2740,8 +3118,11 @@
       <c r="F113" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G113">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2760,8 +3141,11 @@
       <c r="F114" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G114">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2780,8 +3164,11 @@
       <c r="F115" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G115">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2800,8 +3187,11 @@
       <c r="F116" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G116">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2820,8 +3210,11 @@
       <c r="F117" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G117">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2840,8 +3233,11 @@
       <c r="F118" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G118">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2860,8 +3256,11 @@
       <c r="F119" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G119">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2880,8 +3279,11 @@
       <c r="F120" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G120">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2900,8 +3302,11 @@
       <c r="F121" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G121">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2920,8 +3325,11 @@
       <c r="F122" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G122">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2940,8 +3348,11 @@
       <c r="F123" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G123">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2960,8 +3371,11 @@
       <c r="F124" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G124">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2980,8 +3394,11 @@
       <c r="F125" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G125">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -3000,8 +3417,11 @@
       <c r="F126" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G126">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -3020,8 +3440,11 @@
       <c r="F127" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G127">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -3040,8 +3463,11 @@
       <c r="F128" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G128">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -3060,8 +3486,11 @@
       <c r="F129" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G129">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -3080,8 +3509,11 @@
       <c r="F130" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G130">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -3100,8 +3532,11 @@
       <c r="F131" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G131">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -3120,8 +3555,11 @@
       <c r="F132" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G132">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -3140,8 +3578,11 @@
       <c r="F133" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G133">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -3160,8 +3601,11 @@
       <c r="F134" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G134">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -3180,8 +3624,11 @@
       <c r="F135" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G135">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -3200,8 +3647,11 @@
       <c r="F136" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G136">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -3220,8 +3670,11 @@
       <c r="F137" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G137">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -3240,8 +3693,11 @@
       <c r="F138" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G138">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -3260,8 +3716,11 @@
       <c r="F139" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G139">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -3280,8 +3739,11 @@
       <c r="F140" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G140">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -3300,8 +3762,11 @@
       <c r="F141" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G141">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -3320,8 +3785,11 @@
       <c r="F142" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G142">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -3340,8 +3808,11 @@
       <c r="F143" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G143">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -3360,8 +3831,11 @@
       <c r="F144" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G144">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -3380,8 +3854,11 @@
       <c r="F145" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G145">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -3400,8 +3877,11 @@
       <c r="F146" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G146">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -3420,8 +3900,11 @@
       <c r="F147" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G147">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -3440,8 +3923,11 @@
       <c r="F148" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G148">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -3460,8 +3946,11 @@
       <c r="F149" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G149">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -3480,8 +3969,11 @@
       <c r="F150" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G150">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -3500,8 +3992,11 @@
       <c r="F151" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G151">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -3520,8 +4015,11 @@
       <c r="F152" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G152">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -3540,8 +4038,11 @@
       <c r="F153" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G153">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -3560,8 +4061,11 @@
       <c r="F154" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G154">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -3580,8 +4084,11 @@
       <c r="F155" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G155">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -3600,8 +4107,11 @@
       <c r="F156" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G156">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -3620,8 +4130,11 @@
       <c r="F157" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G157">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -3640,8 +4153,11 @@
       <c r="F158" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G158">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -3660,8 +4176,11 @@
       <c r="F159" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G159">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -3680,8 +4199,11 @@
       <c r="F160" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G160">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -3700,8 +4222,11 @@
       <c r="F161" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G161">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -3720,8 +4245,11 @@
       <c r="F162" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G162">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -3740,8 +4268,11 @@
       <c r="F163" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G163">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -3760,8 +4291,11 @@
       <c r="F164" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G164">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -3780,8 +4314,11 @@
       <c r="F165" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G165">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -3800,8 +4337,11 @@
       <c r="F166" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G166">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -3820,8 +4360,11 @@
       <c r="F167" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G167">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -3840,8 +4383,11 @@
       <c r="F168" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G168">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -3860,8 +4406,11 @@
       <c r="F169" s="3">
         <v>11.333333333333334</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G169">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -3880,8 +4429,11 @@
       <c r="F170" s="3">
         <v>11.166666666666666</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G170">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -3900,8 +4452,11 @@
       <c r="F171" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G171">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -3920,8 +4475,11 @@
       <c r="F172" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G172">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -3940,8 +4498,11 @@
       <c r="F173" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G173">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -3960,8 +4521,11 @@
       <c r="F174" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G174">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -3980,8 +4544,11 @@
       <c r="F175" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G175">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -4000,8 +4567,11 @@
       <c r="F176" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G176">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -4020,8 +4590,11 @@
       <c r="F177" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G177">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -4040,8 +4613,11 @@
       <c r="F178" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G178">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -4060,8 +4636,11 @@
       <c r="F179" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G179">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -4080,8 +4659,11 @@
       <c r="F180" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G180">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -4100,8 +4682,11 @@
       <c r="F181" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G181">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -4120,8 +4705,11 @@
       <c r="F182" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G182">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -4140,8 +4728,11 @@
       <c r="F183" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G183">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -4160,8 +4751,11 @@
       <c r="F184" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G184">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -4180,8 +4774,11 @@
       <c r="F185" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G185">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -4200,8 +4797,11 @@
       <c r="F186" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G186">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -4220,8 +4820,11 @@
       <c r="F187" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G187">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -4240,8 +4843,11 @@
       <c r="F188" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G188">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -4260,8 +4866,11 @@
       <c r="F189" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G189">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -4280,8 +4889,11 @@
       <c r="F190" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G190">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -4300,8 +4912,11 @@
       <c r="F191" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G191">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -4320,8 +4935,11 @@
       <c r="F192" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G192">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -4340,8 +4958,11 @@
       <c r="F193" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G193">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -4360,8 +4981,11 @@
       <c r="F194" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G194">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -4380,8 +5004,11 @@
       <c r="F195" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G195">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -4400,8 +5027,11 @@
       <c r="F196" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G196">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -4420,8 +5050,11 @@
       <c r="F197" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G197">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -4440,8 +5073,11 @@
       <c r="F198" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G198">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -4460,8 +5096,11 @@
       <c r="F199" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G199">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -4480,8 +5119,11 @@
       <c r="F200" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G200">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -4500,8 +5142,11 @@
       <c r="F201" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G201">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -4520,8 +5165,11 @@
       <c r="F202" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G202">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -4540,8 +5188,11 @@
       <c r="F203" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G203">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -4560,8 +5211,11 @@
       <c r="F204" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G204">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -4580,8 +5234,11 @@
       <c r="F205" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G205">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -4600,8 +5257,11 @@
       <c r="F206" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G206">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -4620,8 +5280,11 @@
       <c r="F207" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G207">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -4640,8 +5303,11 @@
       <c r="F208" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G208">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -4660,8 +5326,11 @@
       <c r="F209" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G209">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -4680,8 +5349,11 @@
       <c r="F210" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G210">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -4700,8 +5372,11 @@
       <c r="F211" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G211">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -4720,8 +5395,11 @@
       <c r="F212" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G212">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -4740,8 +5418,11 @@
       <c r="F213" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G213">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -4760,8 +5441,11 @@
       <c r="F214" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G214">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -4780,8 +5464,11 @@
       <c r="F215" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G215">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -4799,6 +5486,9 @@
       </c>
       <c r="F216" s="3">
         <v>11</v>
+      </c>
+      <c r="G216">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>